<commit_message>
final commit before adage review
</commit_message>
<xml_diff>
--- a/data/salmon data/data for analysis/Coghill_Wild_Sockeye_final.xlsx
+++ b/data/salmon data/data for analysis/Coghill_Wild_Sockeye_final.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
@@ -993,8 +993,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="215">
+  <cellStyleXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1234,7 +1242,7 @@
     </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="215">
+  <cellStyles count="223">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1342,6 +1350,10 @@
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1449,6 +1461,10 @@
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1780,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="E1:M1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42:M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3297,14 +3313,14 @@
       <c r="J21" s="8">
         <v>0</v>
       </c>
-      <c r="K21" s="13">
-        <v>0</v>
-      </c>
-      <c r="L21" s="13">
-        <v>0</v>
-      </c>
-      <c r="M21" s="13">
-        <v>0</v>
+      <c r="K21" s="8">
+        <v>1</v>
+      </c>
+      <c r="L21" s="8">
+        <v>1</v>
+      </c>
+      <c r="M21" s="8">
+        <v>-1</v>
       </c>
       <c r="N21">
         <v>217115561</v>
@@ -3380,22 +3396,22 @@
         <v>0</v>
       </c>
       <c r="H22" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="8">
-        <v>0</v>
-      </c>
-      <c r="K22" s="13">
-        <v>0</v>
-      </c>
-      <c r="L22" s="13">
-        <v>0</v>
-      </c>
-      <c r="M22" s="13">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0</v>
+      </c>
+      <c r="L22" s="8">
+        <v>1</v>
+      </c>
+      <c r="M22" s="8">
+        <v>-0.94736841999999999</v>
       </c>
       <c r="N22">
         <v>289647730</v>
@@ -3473,19 +3489,19 @@
         <v>0</v>
       </c>
       <c r="I23" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="8">
-        <v>0</v>
-      </c>
-      <c r="K23" s="13">
-        <v>0</v>
-      </c>
-      <c r="L23" s="13">
-        <v>0</v>
-      </c>
-      <c r="M23" s="13">
-        <v>0</v>
+        <v>-0.94736841999999999</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0</v>
+      </c>
+      <c r="L23" s="8">
+        <v>1</v>
+      </c>
+      <c r="M23" s="8">
+        <v>-0.89473683999999998</v>
       </c>
       <c r="N23">
         <v>297246327</v>
@@ -3560,22 +3576,22 @@
         <v>-0.94736841999999999</v>
       </c>
       <c r="H24" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="8">
         <v>1</v>
       </c>
       <c r="J24" s="8">
-        <v>-1</v>
-      </c>
-      <c r="K24" s="13">
-        <v>0</v>
-      </c>
-      <c r="L24" s="13">
-        <v>0</v>
-      </c>
-      <c r="M24" s="13">
-        <v>0</v>
+        <v>-0.89473683999999998</v>
+      </c>
+      <c r="K24" s="8">
+        <v>0</v>
+      </c>
+      <c r="L24" s="8">
+        <v>1</v>
+      </c>
+      <c r="M24" s="8">
+        <v>-0.84210525999999997</v>
       </c>
       <c r="N24">
         <v>532044543</v>
@@ -3656,16 +3672,16 @@
         <v>1</v>
       </c>
       <c r="J25" s="8">
-        <v>-0.94736841999999999</v>
-      </c>
-      <c r="K25" s="13">
-        <v>1</v>
-      </c>
-      <c r="L25" s="13">
-        <v>1</v>
-      </c>
-      <c r="M25" s="13">
-        <v>-1</v>
+        <v>-0.84210525999999997</v>
+      </c>
+      <c r="K25" s="8">
+        <v>0</v>
+      </c>
+      <c r="L25" s="8">
+        <v>1</v>
+      </c>
+      <c r="M25" s="8">
+        <v>-0.78947367999999996</v>
       </c>
       <c r="N25">
         <v>517869725</v>
@@ -3746,16 +3762,16 @@
         <v>1</v>
       </c>
       <c r="J26" s="8">
-        <v>-0.89473683999999998</v>
-      </c>
-      <c r="K26" s="13">
-        <v>0</v>
-      </c>
-      <c r="L26" s="13">
-        <v>1</v>
-      </c>
-      <c r="M26" s="13">
-        <v>-0.94736841999999999</v>
+        <v>-0.78947367999999996</v>
+      </c>
+      <c r="K26" s="8">
+        <v>0</v>
+      </c>
+      <c r="L26" s="8">
+        <v>1</v>
+      </c>
+      <c r="M26" s="8">
+        <v>-0.73684210999999999</v>
       </c>
       <c r="N26">
         <v>617247527</v>
@@ -3836,16 +3852,16 @@
         <v>1</v>
       </c>
       <c r="J27" s="8">
-        <v>-0.84210525999999997</v>
-      </c>
-      <c r="K27" s="13">
-        <v>0</v>
-      </c>
-      <c r="L27" s="13">
-        <v>1</v>
-      </c>
-      <c r="M27" s="13">
-        <v>-0.89473683999999998</v>
+        <v>-0.73684210999999999</v>
+      </c>
+      <c r="K27" s="8">
+        <v>0</v>
+      </c>
+      <c r="L27" s="8">
+        <v>1</v>
+      </c>
+      <c r="M27" s="8">
+        <v>-0.68421052999999998</v>
       </c>
       <c r="N27">
         <v>605425238</v>
@@ -3926,16 +3942,16 @@
         <v>1</v>
       </c>
       <c r="J28" s="8">
-        <v>-0.78947367999999996</v>
-      </c>
-      <c r="K28" s="13">
-        <v>0</v>
-      </c>
-      <c r="L28" s="13">
-        <v>1</v>
-      </c>
-      <c r="M28" s="13">
-        <v>-0.84210525999999997</v>
+        <v>-0.68421052999999998</v>
+      </c>
+      <c r="K28" s="8">
+        <v>0</v>
+      </c>
+      <c r="L28" s="8">
+        <v>1</v>
+      </c>
+      <c r="M28" s="8">
+        <v>-0.63157894999999997</v>
       </c>
       <c r="N28">
         <v>495701890</v>
@@ -4016,16 +4032,16 @@
         <v>1</v>
       </c>
       <c r="J29" s="8">
-        <v>-0.73684210999999999</v>
-      </c>
-      <c r="K29" s="13">
-        <v>0</v>
-      </c>
-      <c r="L29" s="13">
-        <v>1</v>
-      </c>
-      <c r="M29" s="13">
-        <v>-0.78947367999999996</v>
+        <v>-0.63157894999999997</v>
+      </c>
+      <c r="K29" s="8">
+        <v>0</v>
+      </c>
+      <c r="L29" s="8">
+        <v>1</v>
+      </c>
+      <c r="M29" s="8">
+        <v>-0.57894736999999996</v>
       </c>
       <c r="N29">
         <v>567320525</v>
@@ -4106,16 +4122,16 @@
         <v>1</v>
       </c>
       <c r="J30" s="8">
-        <v>-0.68421052999999998</v>
-      </c>
-      <c r="K30" s="13">
-        <v>0</v>
-      </c>
-      <c r="L30" s="13">
-        <v>1</v>
-      </c>
-      <c r="M30" s="13">
-        <v>-0.73684210999999999</v>
+        <v>-0.57894736999999996</v>
+      </c>
+      <c r="K30" s="8">
+        <v>0</v>
+      </c>
+      <c r="L30" s="8">
+        <v>1</v>
+      </c>
+      <c r="M30" s="8">
+        <v>-0.52631578999999995</v>
       </c>
       <c r="N30">
         <v>489220608</v>
@@ -4196,16 +4212,16 @@
         <v>1</v>
       </c>
       <c r="J31" s="8">
-        <v>-0.63157894999999997</v>
-      </c>
-      <c r="K31" s="13">
-        <v>0</v>
-      </c>
-      <c r="L31" s="13">
-        <v>1</v>
-      </c>
-      <c r="M31" s="13">
-        <v>-0.68421052999999998</v>
+        <v>-0.52631578999999995</v>
+      </c>
+      <c r="K31" s="8">
+        <v>0</v>
+      </c>
+      <c r="L31" s="8">
+        <v>1</v>
+      </c>
+      <c r="M31" s="8">
+        <v>-0.47368420999999999</v>
       </c>
       <c r="N31">
         <v>613158229</v>
@@ -4286,16 +4302,16 @@
         <v>1</v>
       </c>
       <c r="J32" s="8">
-        <v>-0.57894736999999996</v>
-      </c>
-      <c r="K32" s="13">
-        <v>0</v>
-      </c>
-      <c r="L32" s="13">
-        <v>1</v>
-      </c>
-      <c r="M32" s="13">
-        <v>-0.63157894999999997</v>
+        <v>-0.47368420999999999</v>
+      </c>
+      <c r="K32" s="8">
+        <v>0</v>
+      </c>
+      <c r="L32" s="8">
+        <v>1</v>
+      </c>
+      <c r="M32" s="8">
+        <v>-0.42105262999999998</v>
       </c>
       <c r="N32">
         <v>641675427</v>
@@ -4376,16 +4392,16 @@
         <v>1</v>
       </c>
       <c r="J33" s="8">
-        <v>-0.52631578999999995</v>
-      </c>
-      <c r="K33" s="13">
-        <v>0</v>
-      </c>
-      <c r="L33" s="13">
-        <v>1</v>
-      </c>
-      <c r="M33" s="13">
-        <v>-0.57894736999999996</v>
+        <v>-0.42105262999999998</v>
+      </c>
+      <c r="K33" s="8">
+        <v>0</v>
+      </c>
+      <c r="L33" s="8">
+        <v>1</v>
+      </c>
+      <c r="M33" s="8">
+        <v>-0.36842105000000003</v>
       </c>
       <c r="N33">
         <v>483704011</v>
@@ -4466,16 +4482,16 @@
         <v>1</v>
       </c>
       <c r="J34" s="8">
-        <v>-0.47368420999999999</v>
-      </c>
-      <c r="K34" s="13">
-        <v>0</v>
-      </c>
-      <c r="L34" s="13">
-        <v>1</v>
-      </c>
-      <c r="M34" s="13">
-        <v>-0.52631578999999995</v>
+        <v>-0.36842105000000003</v>
+      </c>
+      <c r="K34" s="8">
+        <v>0</v>
+      </c>
+      <c r="L34" s="8">
+        <v>1</v>
+      </c>
+      <c r="M34" s="8">
+        <v>-0.31578947000000002</v>
       </c>
       <c r="N34">
         <v>542383070</v>
@@ -4556,16 +4572,16 @@
         <v>1</v>
       </c>
       <c r="J35" s="8">
-        <v>-0.42105262999999998</v>
-      </c>
-      <c r="K35" s="13">
-        <v>0</v>
-      </c>
-      <c r="L35" s="13">
-        <v>1</v>
-      </c>
-      <c r="M35" s="13">
-        <v>-0.47368420999999999</v>
+        <v>-0.31578947000000002</v>
+      </c>
+      <c r="K35" s="8">
+        <v>0</v>
+      </c>
+      <c r="L35" s="8">
+        <v>1</v>
+      </c>
+      <c r="M35" s="8">
+        <v>-0.26315789000000001</v>
       </c>
       <c r="N35">
         <v>602128903</v>
@@ -4646,16 +4662,16 @@
         <v>1</v>
       </c>
       <c r="J36" s="8">
-        <v>-0.36842105000000003</v>
-      </c>
-      <c r="K36" s="13">
-        <v>0</v>
-      </c>
-      <c r="L36" s="13">
-        <v>1</v>
-      </c>
-      <c r="M36" s="13">
-        <v>-0.42105262999999998</v>
+        <v>-0.26315789000000001</v>
+      </c>
+      <c r="K36" s="8">
+        <v>0</v>
+      </c>
+      <c r="L36" s="8">
+        <v>1</v>
+      </c>
+      <c r="M36" s="8">
+        <v>-0.21052631999999999</v>
       </c>
       <c r="N36">
         <v>586607038</v>
@@ -4736,16 +4752,16 @@
         <v>1</v>
       </c>
       <c r="J37" s="8">
-        <v>-0.31578947000000002</v>
-      </c>
-      <c r="K37" s="13">
-        <v>0</v>
-      </c>
-      <c r="L37" s="13">
-        <v>1</v>
-      </c>
-      <c r="M37" s="13">
-        <v>-0.36842105000000003</v>
+        <v>-0.21052631999999999</v>
+      </c>
+      <c r="K37" s="8">
+        <v>0</v>
+      </c>
+      <c r="L37" s="8">
+        <v>1</v>
+      </c>
+      <c r="M37" s="8">
+        <v>-0.15789474000000001</v>
       </c>
       <c r="N37">
         <v>621062096</v>
@@ -4826,16 +4842,16 @@
         <v>1</v>
       </c>
       <c r="J38" s="8">
-        <v>-0.26315789000000001</v>
-      </c>
-      <c r="K38" s="13">
-        <v>0</v>
-      </c>
-      <c r="L38" s="13">
-        <v>1</v>
-      </c>
-      <c r="M38" s="13">
-        <v>-0.31578947000000002</v>
+        <v>-0.15789474000000001</v>
+      </c>
+      <c r="K38" s="8">
+        <v>0</v>
+      </c>
+      <c r="L38" s="8">
+        <v>1</v>
+      </c>
+      <c r="M38" s="8">
+        <v>-0.10526315999999999</v>
       </c>
       <c r="N38">
         <v>603754659</v>
@@ -4916,16 +4932,16 @@
         <v>1</v>
       </c>
       <c r="J39" s="8">
-        <v>-0.21052631999999999</v>
-      </c>
-      <c r="K39" s="13">
-        <v>0</v>
-      </c>
-      <c r="L39" s="13">
-        <v>1</v>
-      </c>
-      <c r="M39" s="13">
-        <v>-0.26315789000000001</v>
+        <v>-0.10526315999999999</v>
+      </c>
+      <c r="K39" s="8">
+        <v>0</v>
+      </c>
+      <c r="L39" s="8">
+        <v>1</v>
+      </c>
+      <c r="M39" s="8">
+        <v>-5.2631579999999997E-2</v>
       </c>
       <c r="N39">
         <v>607943252</v>
@@ -5006,16 +5022,16 @@
         <v>1</v>
       </c>
       <c r="J40" s="8">
-        <v>-0.15789474000000001</v>
-      </c>
-      <c r="K40" s="13">
-        <v>0</v>
-      </c>
-      <c r="L40" s="13">
-        <v>1</v>
-      </c>
-      <c r="M40" s="13">
-        <v>-0.21052631999999999</v>
+        <v>-5.2631579999999997E-2</v>
+      </c>
+      <c r="K40" s="8">
+        <v>0</v>
+      </c>
+      <c r="L40" s="8">
+        <v>1</v>
+      </c>
+      <c r="M40" s="8">
+        <v>0</v>
       </c>
       <c r="N40">
         <v>638846859</v>
@@ -5096,16 +5112,16 @@
         <v>1</v>
       </c>
       <c r="J41" s="8">
-        <v>-0.10526315999999999</v>
-      </c>
-      <c r="K41" s="13">
-        <v>0</v>
-      </c>
-      <c r="L41" s="13">
-        <v>1</v>
-      </c>
-      <c r="M41" s="13">
-        <v>-0.15789474000000001</v>
+        <v>0</v>
+      </c>
+      <c r="K41" s="8">
+        <v>0</v>
+      </c>
+      <c r="L41" s="8">
+        <v>1</v>
+      </c>
+      <c r="M41" s="8">
+        <v>0</v>
       </c>
       <c r="N41">
         <v>564053077</v>
@@ -5186,16 +5202,16 @@
         <v>1</v>
       </c>
       <c r="J42" s="8">
-        <v>-5.2631579999999997E-2</v>
-      </c>
-      <c r="K42" s="13">
-        <v>0</v>
-      </c>
-      <c r="L42" s="13">
-        <v>1</v>
-      </c>
-      <c r="M42" s="13">
-        <v>-0.10526315999999999</v>
+        <v>0</v>
+      </c>
+      <c r="K42" s="8">
+        <v>0</v>
+      </c>
+      <c r="L42" s="8">
+        <v>1</v>
+      </c>
+      <c r="M42" s="8">
+        <v>0</v>
       </c>
       <c r="N42">
         <v>599490314</v>
@@ -5262,6 +5278,9 @@
       <c r="F43" s="8">
         <v>1</v>
       </c>
+      <c r="G43" s="8">
+        <v>0</v>
+      </c>
       <c r="H43" s="8">
         <v>0</v>
       </c>
@@ -5271,14 +5290,14 @@
       <c r="J43" s="8">
         <v>0</v>
       </c>
-      <c r="K43" s="13">
-        <v>0</v>
-      </c>
-      <c r="L43" s="13">
-        <v>1</v>
-      </c>
-      <c r="M43" s="13">
-        <v>-5.2631579999999997E-2</v>
+      <c r="K43" s="8">
+        <v>0</v>
+      </c>
+      <c r="L43" s="8">
+        <v>1</v>
+      </c>
+      <c r="M43" s="8">
+        <v>0</v>
       </c>
       <c r="N43">
         <v>617608302</v>
@@ -5345,19 +5364,25 @@
       <c r="F44" s="8">
         <v>1</v>
       </c>
+      <c r="G44" s="8">
+        <v>0</v>
+      </c>
       <c r="H44" s="8">
         <v>0</v>
       </c>
       <c r="I44" s="8">
         <v>1</v>
       </c>
-      <c r="K44" s="13">
-        <v>0</v>
-      </c>
-      <c r="L44" s="13">
-        <v>1</v>
-      </c>
-      <c r="M44" s="13">
+      <c r="J44" s="8">
+        <v>0</v>
+      </c>
+      <c r="K44" s="8">
+        <v>0</v>
+      </c>
+      <c r="L44" s="8">
+        <v>1</v>
+      </c>
+      <c r="M44" s="8">
         <v>0</v>
       </c>
       <c r="N44">
@@ -5425,19 +5450,27 @@
       <c r="F45" s="8">
         <v>1</v>
       </c>
+      <c r="G45" s="8">
+        <v>0</v>
+      </c>
       <c r="H45" s="8">
         <v>0</v>
       </c>
       <c r="I45" s="8">
         <v>1</v>
       </c>
-      <c r="K45" s="13">
-        <v>0</v>
-      </c>
-      <c r="L45" s="13">
-        <v>1</v>
-      </c>
-      <c r="M45" s="13"/>
+      <c r="J45" s="8">
+        <v>0</v>
+      </c>
+      <c r="K45" s="8">
+        <v>0</v>
+      </c>
+      <c r="L45" s="8">
+        <v>1</v>
+      </c>
+      <c r="M45" s="8">
+        <v>0</v>
+      </c>
       <c r="N45">
         <v>640202598</v>
       </c>
@@ -5497,19 +5530,27 @@
       <c r="F46" s="8">
         <v>1</v>
       </c>
+      <c r="G46" s="8">
+        <v>0</v>
+      </c>
       <c r="H46" s="8">
         <v>0</v>
       </c>
       <c r="I46" s="8">
         <v>1</v>
       </c>
-      <c r="K46" s="13">
-        <v>0</v>
-      </c>
-      <c r="L46" s="13">
-        <v>1</v>
-      </c>
-      <c r="M46" s="13"/>
+      <c r="J46" s="8">
+        <v>0</v>
+      </c>
+      <c r="K46" s="8">
+        <v>0</v>
+      </c>
+      <c r="L46" s="8">
+        <v>1</v>
+      </c>
+      <c r="M46" s="8">
+        <v>0</v>
+      </c>
       <c r="N46">
         <v>647083753</v>
       </c>
@@ -5563,19 +5604,27 @@
       <c r="F47" s="8">
         <v>1</v>
       </c>
+      <c r="G47" s="8">
+        <v>0</v>
+      </c>
       <c r="H47" s="8">
         <v>0</v>
       </c>
       <c r="I47" s="8">
         <v>1</v>
       </c>
-      <c r="K47" s="13">
-        <v>0</v>
-      </c>
-      <c r="L47" s="13">
-        <v>1</v>
-      </c>
-      <c r="M47" s="13"/>
+      <c r="J47" s="8">
+        <v>0</v>
+      </c>
+      <c r="K47" s="8">
+        <v>0</v>
+      </c>
+      <c r="L47" s="8">
+        <v>1</v>
+      </c>
+      <c r="M47" s="8">
+        <v>0</v>
+      </c>
       <c r="N47">
         <v>641603439</v>
       </c>
@@ -5621,19 +5670,27 @@
       <c r="F48" s="8">
         <v>1</v>
       </c>
+      <c r="G48" s="8">
+        <v>0</v>
+      </c>
       <c r="H48" s="8">
         <v>0</v>
       </c>
       <c r="I48" s="8">
         <v>1</v>
       </c>
-      <c r="K48" s="13">
-        <v>0</v>
-      </c>
-      <c r="L48" s="13">
-        <v>1</v>
-      </c>
-      <c r="M48" s="13"/>
+      <c r="J48" s="8">
+        <v>0</v>
+      </c>
+      <c r="K48" s="8">
+        <v>0</v>
+      </c>
+      <c r="L48" s="8">
+        <v>1</v>
+      </c>
+      <c r="M48" s="8">
+        <v>0</v>
+      </c>
       <c r="N48">
         <v>673526737</v>
       </c>
@@ -5658,9 +5715,7 @@
       </c>
       <c r="W48" s="15"/>
     </row>
-    <row r="49" spans="11:23">
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
+    <row r="49" spans="13:23">
       <c r="M49" s="13"/>
       <c r="N49"/>
       <c r="O49"/>
@@ -5671,16 +5726,14 @@
       <c r="U49"/>
       <c r="W49" s="15"/>
     </row>
-    <row r="50" spans="11:23">
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
+    <row r="50" spans="13:23">
       <c r="M50" s="13"/>
       <c r="N50"/>
       <c r="O50"/>
       <c r="P50"/>
       <c r="W50" s="15"/>
     </row>
-    <row r="51" spans="11:23">
+    <row r="51" spans="13:23">
       <c r="W51" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Coghill Lake data
</commit_message>
<xml_diff>
--- a/data/salmon data/data for analysis/Coghill_Wild_Sockeye_final.xlsx
+++ b/data/salmon data/data for analysis/Coghill_Wild_Sockeye_final.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="1480" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -867,7 +867,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -981,8 +981,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -995,8 +1001,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCF305"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1004,6 +1016,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1232,7 +1255,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1256,6 +1279,10 @@
     </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="225">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1811,17 +1838,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH51"/>
+  <dimension ref="A1:AH48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AB49"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="22" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="8" customWidth="1"/>
     <col min="5" max="18" width="11" style="8" customWidth="1"/>
     <col min="19" max="19" width="11" style="14" customWidth="1"/>
@@ -1932,12 +1959,12 @@
       <c r="B2" s="3">
         <v>11800</v>
       </c>
-      <c r="C2" s="8">
-        <v>87325</v>
+      <c r="C2" s="19">
+        <v>137510</v>
       </c>
       <c r="D2" s="8">
         <f>C2/B2</f>
-        <v>7.4004237288135597</v>
+        <v>11.653389830508475</v>
       </c>
       <c r="E2" s="8">
         <v>0</v>
@@ -1982,12 +2009,12 @@
       <c r="B3" s="3">
         <v>81000</v>
       </c>
-      <c r="C3" s="8">
-        <v>159288</v>
+      <c r="C3" s="19">
+        <v>91750</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" ref="D3:D42" si="0">C3/B3</f>
-        <v>1.9665185185185186</v>
+        <v>1.132716049382716</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -2044,12 +2071,12 @@
       <c r="B4" s="3">
         <v>35200</v>
       </c>
-      <c r="C4" s="8">
-        <v>62559.000000000007</v>
+      <c r="C4" s="19">
+        <v>220868</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="0"/>
-        <v>1.7772443181818185</v>
+        <v>6.2746590909090907</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -2113,12 +2140,12 @@
       <c r="B5" s="3">
         <v>15000</v>
       </c>
-      <c r="C5" s="8">
-        <v>60516</v>
+      <c r="C5" s="19">
+        <v>46728</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="0"/>
-        <v>4.0343999999999998</v>
+        <v>3.1152000000000002</v>
       </c>
       <c r="E5" s="8">
         <v>0</v>
@@ -2182,12 +2209,12 @@
       <c r="B6" s="3">
         <v>51000</v>
       </c>
-      <c r="C6" s="8">
-        <v>184971.16932856577</v>
+      <c r="C6" s="19">
+        <v>218570</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
-        <v>3.6268856731091326</v>
+        <v>4.2856862745098043</v>
       </c>
       <c r="E6" s="8">
         <v>0</v>
@@ -2251,12 +2278,12 @@
       <c r="B7" s="3">
         <v>55000</v>
       </c>
-      <c r="C7" s="8">
-        <v>132283.99999999951</v>
+      <c r="C7" s="19">
+        <v>233690</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
-        <v>2.4051636363636275</v>
+        <v>4.2489090909090912</v>
       </c>
       <c r="E7" s="8">
         <v>0</v>
@@ -2321,12 +2348,12 @@
       <c r="B8" s="3">
         <v>22334</v>
       </c>
-      <c r="C8" s="8">
-        <v>121757</v>
+      <c r="C8" s="19">
+        <v>110825</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="0"/>
-        <v>5.4516432345303123</v>
+        <v>4.9621653084982542</v>
       </c>
       <c r="E8" s="8">
         <v>0</v>
@@ -2392,12 +2419,12 @@
       <c r="B9" s="3">
         <v>34855</v>
       </c>
-      <c r="C9" s="8">
-        <v>182706</v>
+      <c r="C9" s="19">
+        <v>191530</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="0"/>
-        <v>5.2418878209726012</v>
+        <v>5.4950509252617987</v>
       </c>
       <c r="E9" s="8">
         <v>0</v>
@@ -2465,12 +2492,12 @@
       <c r="B10" s="3">
         <v>9056</v>
       </c>
-      <c r="C10" s="8">
-        <v>69421</v>
+      <c r="C10" s="19">
+        <v>173531</v>
       </c>
       <c r="D10" s="8">
         <f t="shared" si="0"/>
-        <v>7.665746466431095</v>
+        <v>19.161992049469966</v>
       </c>
       <c r="E10" s="8">
         <v>0</v>
@@ -2540,12 +2567,12 @@
       <c r="B11" s="3">
         <v>31562</v>
       </c>
-      <c r="C11" s="8">
-        <v>202340</v>
+      <c r="C11" s="19">
+        <v>1251048</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" si="0"/>
-        <v>6.4108738356251189</v>
+        <v>39.637792281857934</v>
       </c>
       <c r="E11" s="8">
         <v>0</v>
@@ -2615,12 +2642,12 @@
       <c r="B12" s="3">
         <v>42284</v>
       </c>
-      <c r="C12" s="8">
-        <v>245808</v>
+      <c r="C12" s="19">
+        <v>70303</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="0"/>
-        <v>5.813262699839183</v>
+        <v>1.6626383502033866</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
@@ -2690,12 +2717,12 @@
       <c r="B13" s="3">
         <v>48281</v>
       </c>
-      <c r="C13" s="8">
-        <v>126991</v>
+      <c r="C13" s="19">
+        <v>150407</v>
       </c>
       <c r="D13" s="8">
         <f t="shared" si="0"/>
-        <v>2.6302479236138439</v>
+        <v>3.115242020670657</v>
       </c>
       <c r="E13" s="8">
         <v>0</v>
@@ -2769,12 +2796,12 @@
       <c r="B14" s="3">
         <v>142253</v>
       </c>
-      <c r="C14" s="8">
-        <v>201386.99999999997</v>
+      <c r="C14" s="19">
+        <v>473656</v>
       </c>
       <c r="D14" s="8">
         <f t="shared" si="0"/>
-        <v>1.4156959782921974</v>
+        <v>3.3296731879116783</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
@@ -2855,12 +2882,12 @@
       <c r="B15" s="3">
         <v>156112</v>
       </c>
-      <c r="C15" s="8">
-        <v>259166.99999999991</v>
+      <c r="C15" s="19">
+        <v>496238</v>
       </c>
       <c r="D15" s="8">
         <f t="shared" si="0"/>
-        <v>1.6601350312596079</v>
+        <v>3.1787306549144203</v>
       </c>
       <c r="E15" s="8">
         <v>0</v>
@@ -2949,12 +2976,12 @@
       <c r="B16" s="3">
         <v>180314</v>
       </c>
-      <c r="C16" s="8">
-        <v>1127475.2720999999</v>
+      <c r="C16" s="19">
+        <v>612159</v>
       </c>
       <c r="D16" s="8">
         <f t="shared" si="0"/>
-        <v>6.2528437730847299</v>
+        <v>3.394961012456049</v>
       </c>
       <c r="E16" s="8">
         <v>0</v>
@@ -3043,12 +3070,12 @@
       <c r="B17" s="3">
         <v>38783</v>
       </c>
-      <c r="C17" s="8">
-        <v>73025</v>
+      <c r="C17" s="19">
+        <v>106297</v>
       </c>
       <c r="D17" s="8">
         <f t="shared" si="0"/>
-        <v>1.8829126163525256</v>
+        <v>2.7408142742954387</v>
       </c>
       <c r="E17" s="8">
         <v>0</v>
@@ -3139,12 +3166,12 @@
       <c r="B18" s="3">
         <v>63622</v>
       </c>
-      <c r="C18" s="8">
-        <v>157245</v>
+      <c r="C18" s="19">
+        <v>203086</v>
       </c>
       <c r="D18" s="8">
         <f t="shared" si="0"/>
-        <v>2.4715507214485557</v>
+        <v>3.1920719248058846</v>
       </c>
       <c r="E18" s="8">
         <v>0</v>
@@ -3233,12 +3260,12 @@
       <c r="B19" s="3">
         <v>163342</v>
       </c>
-      <c r="C19" s="8">
-        <v>509273.83158215007</v>
+      <c r="C19" s="19">
+        <v>16598</v>
       </c>
       <c r="D19" s="8">
         <f t="shared" si="0"/>
-        <v>3.1178376142213886</v>
+        <v>0.10161501634607144</v>
       </c>
       <c r="E19" s="8">
         <v>0</v>
@@ -3330,12 +3357,12 @@
       <c r="B20" s="3">
         <v>74135</v>
       </c>
-      <c r="C20" s="8">
-        <v>469304.65756999992</v>
+      <c r="C20" s="19">
+        <v>26918</v>
       </c>
       <c r="D20" s="8">
         <f t="shared" si="0"/>
-        <v>6.3304061181628102</v>
+        <v>0.36309435489310043</v>
       </c>
       <c r="E20" s="8">
         <v>0</v>
@@ -3425,12 +3452,12 @@
       <c r="B21" s="3">
         <v>187263</v>
       </c>
-      <c r="C21" s="8">
-        <v>598733</v>
+      <c r="C21" s="19">
+        <v>60053</v>
       </c>
       <c r="D21" s="8">
         <f t="shared" si="0"/>
-        <v>3.1972840336852446</v>
+        <v>0.32068801631929428</v>
       </c>
       <c r="E21" s="8">
         <v>0</v>
@@ -3522,12 +3549,12 @@
       <c r="B22" s="3">
         <v>72023</v>
       </c>
-      <c r="C22" s="8">
-        <v>152650</v>
+      <c r="C22" s="19">
+        <v>50495</v>
       </c>
       <c r="D22" s="8">
         <f t="shared" si="0"/>
-        <v>2.1194618385793427</v>
+        <v>0.70109548338725125</v>
       </c>
       <c r="E22" s="8">
         <v>0</v>
@@ -3618,12 +3645,12 @@
       <c r="B23" s="3">
         <v>36881</v>
       </c>
-      <c r="C23" s="8">
-        <v>144785</v>
+      <c r="C23" s="19">
+        <v>9410</v>
       </c>
       <c r="D23" s="8">
         <f t="shared" si="0"/>
-        <v>3.9257341178384535</v>
+        <v>0.25514492557143242</v>
       </c>
       <c r="E23" s="8">
         <v>1</v>
@@ -3714,12 +3741,12 @@
       <c r="B24" s="3">
         <v>8250</v>
       </c>
-      <c r="C24" s="8">
-        <v>19620.419999999998</v>
+      <c r="C24" s="19">
+        <v>26127</v>
       </c>
       <c r="D24" s="8">
         <f t="shared" si="0"/>
-        <v>2.3782327272727271</v>
+        <v>3.1669090909090909</v>
       </c>
       <c r="E24" s="8">
         <v>0</v>
@@ -3810,12 +3837,12 @@
       <c r="B25" s="3">
         <v>9701</v>
       </c>
-      <c r="C25" s="8">
-        <v>20302.158845587157</v>
+      <c r="C25" s="19">
+        <v>153809</v>
       </c>
       <c r="D25" s="8">
         <f t="shared" si="0"/>
-        <v>2.0927903149765132</v>
+        <v>15.85496340583445</v>
       </c>
       <c r="E25" s="8">
         <v>0</v>
@@ -3906,12 +3933,12 @@
       <c r="B26" s="3">
         <v>29642</v>
       </c>
-      <c r="C26" s="8">
-        <v>67203.278000000006</v>
+      <c r="C26" s="19">
+        <v>114128</v>
       </c>
       <c r="D26" s="8">
         <f t="shared" si="0"/>
-        <v>2.2671640914918023</v>
+        <v>3.8502125362661088</v>
       </c>
       <c r="E26" s="8">
         <v>0</v>
@@ -4002,12 +4029,12 @@
       <c r="B27" s="3">
         <v>9232</v>
       </c>
-      <c r="C27" s="8">
-        <v>48357</v>
+      <c r="C27" s="19">
+        <v>67501</v>
       </c>
       <c r="D27" s="8">
         <f t="shared" si="0"/>
-        <v>5.2379766031195842</v>
+        <v>7.3116334488734838</v>
       </c>
       <c r="E27" s="8">
         <v>0</v>
@@ -4098,12 +4125,12 @@
       <c r="B28" s="3">
         <v>7264</v>
       </c>
-      <c r="C28" s="8">
-        <v>9291</v>
+      <c r="C28" s="19">
+        <v>27941</v>
       </c>
       <c r="D28" s="8">
         <f t="shared" si="0"/>
-        <v>1.2790473568281939</v>
+        <v>3.8465033039647576</v>
       </c>
       <c r="E28" s="8">
         <v>0</v>
@@ -4194,12 +4221,12 @@
       <c r="B29" s="3">
         <v>30382</v>
       </c>
-      <c r="C29" s="8">
-        <v>61296</v>
+      <c r="C29" s="19">
+        <v>317407</v>
       </c>
       <c r="D29" s="8">
         <f t="shared" si="0"/>
-        <v>2.0175103679810413</v>
+        <v>10.44720558225265</v>
       </c>
       <c r="E29" s="8">
         <v>0</v>
@@ -4290,12 +4317,12 @@
       <c r="B30" s="3">
         <v>38693</v>
       </c>
-      <c r="C30" s="8">
-        <v>131181</v>
+      <c r="C30" s="19">
+        <v>133377</v>
       </c>
       <c r="D30" s="8">
         <f t="shared" si="0"/>
-        <v>3.390303155609542</v>
+        <v>3.4470576073191532</v>
       </c>
       <c r="E30" s="8">
         <v>0</v>
@@ -4386,12 +4413,12 @@
       <c r="B31" s="3">
         <v>35010</v>
       </c>
-      <c r="C31" s="8">
-        <v>106750.98300000001</v>
+      <c r="C31" s="19">
+        <v>44736</v>
       </c>
       <c r="D31" s="8">
         <f t="shared" si="0"/>
-        <v>3.0491568980291346</v>
+        <v>1.2778063410454157</v>
       </c>
       <c r="E31" s="8">
         <v>0</v>
@@ -4482,12 +4509,12 @@
       <c r="B32" s="3">
         <v>28963</v>
       </c>
-      <c r="C32" s="8">
-        <v>63370</v>
+      <c r="C32" s="19">
+        <v>89490</v>
       </c>
       <c r="D32" s="8">
         <f t="shared" si="0"/>
-        <v>2.1879639540102889</v>
+        <v>3.0898042329869142</v>
       </c>
       <c r="E32" s="8">
         <v>0</v>
@@ -4578,12 +4605,12 @@
       <c r="B33" s="3">
         <v>59311</v>
       </c>
-      <c r="C33" s="8">
-        <v>148052</v>
+      <c r="C33" s="19">
+        <v>234831</v>
       </c>
       <c r="D33" s="8">
         <f t="shared" si="0"/>
-        <v>2.4961980071150376</v>
+        <v>3.9593161470890728</v>
       </c>
       <c r="E33" s="8">
         <v>0</v>
@@ -4674,12 +4701,12 @@
       <c r="B34" s="3">
         <v>28416</v>
       </c>
-      <c r="C34" s="8">
-        <v>213816</v>
+      <c r="C34" s="19">
+        <v>143849</v>
       </c>
       <c r="D34" s="8">
         <f t="shared" si="0"/>
-        <v>7.524493243243243</v>
+        <v>5.0622536599099099</v>
       </c>
       <c r="E34" s="8">
         <v>0</v>
@@ -4770,12 +4797,12 @@
       <c r="B35" s="3">
         <v>38547</v>
       </c>
-      <c r="C35" s="8">
-        <v>126026</v>
+      <c r="C35" s="20">
+        <v>15616</v>
       </c>
       <c r="D35" s="8">
         <f t="shared" si="0"/>
-        <v>3.2694113679404362</v>
+        <v>0.40511583261991851</v>
       </c>
       <c r="E35" s="8">
         <v>0</v>
@@ -4866,12 +4893,12 @@
       <c r="B36" s="3">
         <v>28323</v>
       </c>
-      <c r="C36" s="8">
-        <v>52603</v>
+      <c r="C36" s="19">
+        <v>180332</v>
       </c>
       <c r="D36" s="8">
         <f t="shared" si="0"/>
-        <v>1.8572538219821346</v>
+        <v>6.3669808989160757</v>
       </c>
       <c r="E36" s="8">
         <v>0</v>
@@ -4962,12 +4989,12 @@
       <c r="B37" s="3">
         <v>75427</v>
       </c>
-      <c r="C37" s="8">
-        <v>170013</v>
+      <c r="C37" s="19">
+        <v>102397</v>
       </c>
       <c r="D37" s="8">
         <f t="shared" si="0"/>
-        <v>2.2540071857557638</v>
+        <v>1.3575642674373898</v>
       </c>
       <c r="E37" s="8">
         <v>0</v>
@@ -5058,12 +5085,12 @@
       <c r="B38" s="3">
         <v>30569</v>
       </c>
-      <c r="C38" s="8">
-        <v>190475</v>
+      <c r="C38" s="19">
+        <v>154110</v>
       </c>
       <c r="D38" s="8">
         <f t="shared" si="0"/>
-        <v>6.230985639046092</v>
+        <v>5.0413817920115154</v>
       </c>
       <c r="E38" s="8">
         <v>0</v>
@@ -5154,12 +5181,12 @@
       <c r="B39" s="3">
         <v>30313</v>
       </c>
-      <c r="C39" s="8">
-        <v>94282</v>
+      <c r="C39" s="19">
+        <v>35754</v>
       </c>
       <c r="D39" s="8">
         <f t="shared" si="0"/>
-        <v>3.1102827169861116</v>
+        <v>1.1794939464916043</v>
       </c>
       <c r="E39" s="8">
         <v>0</v>
@@ -5250,12 +5277,12 @@
       <c r="B40" s="3">
         <v>23479</v>
       </c>
-      <c r="C40" s="8">
-        <v>32870</v>
+      <c r="C40" s="19">
+        <v>164495</v>
       </c>
       <c r="D40" s="8">
         <f t="shared" si="0"/>
-        <v>1.3999744452489458</v>
+        <v>7.0060479577494785</v>
       </c>
       <c r="E40" s="8">
         <v>0</v>
@@ -5346,12 +5373,12 @@
       <c r="B41" s="3">
         <v>70001</v>
       </c>
-      <c r="C41" s="8">
-        <v>183026</v>
+      <c r="C41" s="19">
+        <v>649042</v>
       </c>
       <c r="D41" s="8">
         <f t="shared" si="0"/>
-        <v>2.6146197911458406</v>
+        <v>9.2718961157697741</v>
       </c>
       <c r="E41" s="8">
         <v>0</v>
@@ -5442,12 +5469,12 @@
       <c r="B42" s="3">
         <v>29298</v>
       </c>
-      <c r="C42" s="8">
-        <v>120574</v>
+      <c r="C42" s="19">
+        <v>71784</v>
       </c>
       <c r="D42" s="8">
         <f t="shared" si="0"/>
-        <v>4.115434500648508</v>
+        <v>2.4501331148883883</v>
       </c>
       <c r="E42" s="8">
         <v>0</v>
@@ -5538,8 +5565,8 @@
       <c r="B43" s="4">
         <v>23186</v>
       </c>
-      <c r="C43" s="8">
-        <v>113040</v>
+      <c r="C43" s="19">
+        <v>120904</v>
       </c>
       <c r="E43" s="8">
         <v>0</v>
@@ -5630,8 +5657,8 @@
       <c r="B44" s="4">
         <v>24312</v>
       </c>
-      <c r="C44" s="8">
-        <v>66793</v>
+      <c r="C44" s="19">
+        <v>21034</v>
       </c>
       <c r="E44" s="8">
         <v>0</v>
@@ -5722,8 +5749,8 @@
       <c r="B45" s="12">
         <v>102359</v>
       </c>
-      <c r="C45" s="8">
-        <v>234022</v>
+      <c r="C45" s="21">
+        <v>199</v>
       </c>
       <c r="E45" s="8">
         <v>0</v>
@@ -5808,9 +5835,6 @@
       <c r="B46" s="12">
         <v>74978</v>
       </c>
-      <c r="C46" s="8">
-        <v>573938</v>
-      </c>
       <c r="E46" s="8">
         <v>0</v>
       </c>
@@ -5888,9 +5912,6 @@
       <c r="B47" s="12">
         <v>17231</v>
       </c>
-      <c r="C47" s="8">
-        <v>79944</v>
-      </c>
       <c r="E47" s="8">
         <v>0</v>
       </c>
@@ -5960,9 +5981,6 @@
       <c r="B48" s="12">
         <v>21836</v>
       </c>
-      <c r="C48" s="8">
-        <v>104806</v>
-      </c>
       <c r="E48" s="8">
         <v>0</v>
       </c>
@@ -6015,29 +6033,6 @@
       <c r="W48" s="15"/>
       <c r="AA48" s="14"/>
       <c r="AB48" s="14"/>
-    </row>
-    <row r="49" spans="13:28">
-      <c r="M49" s="13"/>
-      <c r="N49"/>
-      <c r="O49"/>
-      <c r="P49"/>
-      <c r="Q49">
-        <v>2329059.6330275228</v>
-      </c>
-      <c r="U49"/>
-      <c r="W49" s="15"/>
-      <c r="AA49" s="14"/>
-      <c r="AB49" s="14"/>
-    </row>
-    <row r="50" spans="13:28">
-      <c r="M50" s="13"/>
-      <c r="N50"/>
-      <c r="O50"/>
-      <c r="P50"/>
-      <c r="W50" s="15"/>
-    </row>
-    <row r="51" spans="13:28">
-      <c r="W51" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>